<commit_message>
-Warehouse inventory -Reading Orders
</commit_message>
<xml_diff>
--- a/Documents/Book1.xlsx
+++ b/Documents/Book1.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="permissions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="61">
   <si>
     <t>دوربین</t>
   </si>
@@ -175,13 +177,46 @@
   </si>
   <si>
     <t>credit</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>new duty</t>
+  </si>
+  <si>
+    <t>sent items</t>
+  </si>
+  <si>
+    <t>asset received</t>
+  </si>
+  <si>
+    <t>edit order</t>
+  </si>
+  <si>
+    <t>remove order</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Add a new</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>venue_owner</t>
+  </si>
+  <si>
+    <t>record_owner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,16 +224,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFC3CEE3"/>
+      <name val="Fira Code"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -380,11 +433,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -407,6 +622,77 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,11 +975,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -706,7 +992,7 @@
     <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -720,7 +1006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -734,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -766,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -799,7 +1085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -832,7 +1118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -865,7 +1151,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="M9" s="2">
         <v>4</v>
       </c>
@@ -876,7 +1162,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -899,7 +1185,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -922,7 +1208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -954,7 +1240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -978,7 +1264,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -1002,7 +1288,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -1026,7 +1312,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1054,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1086,7 +1372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1110,7 +1396,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -1134,7 +1420,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="3">
         <v>3</v>
       </c>
@@ -1171,7 +1457,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
@@ -1180,7 +1466,7 @@
     <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1194,7 +1480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1208,10 +1494,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
@@ -1237,7 +1523,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -1263,7 +1549,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -1289,7 +1575,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1315,7 +1601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -1341,7 +1627,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -1367,7 +1653,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -1393,7 +1679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -1419,7 +1705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="A12" s="6">
         <v>8</v>
       </c>
@@ -1443,6 +1729,592 @@
       </c>
       <c r="H12" s="8" t="s">
         <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A1" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="29"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16">
+        <v>0</v>
+      </c>
+      <c r="K2" s="29"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="29"/>
+      <c r="M5" s="30"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="29"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A1" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="35">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36">
+        <v>0</v>
+      </c>
+      <c r="D2" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="38">
+        <v>0</v>
+      </c>
+      <c r="C3" s="39">
+        <v>1</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="38">
+        <v>0</v>
+      </c>
+      <c r="C4" s="39">
+        <v>1</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="38">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39">
+        <v>1</v>
+      </c>
+      <c r="D5" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="41">
+        <v>1</v>
+      </c>
+      <c r="C6" s="42">
+        <v>0</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="41">
+        <v>1</v>
+      </c>
+      <c r="C7" s="39">
+        <v>1</v>
+      </c>
+      <c r="D7" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="38">
+        <v>0</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0</v>
+      </c>
+      <c r="D8" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A9" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="45">
+        <v>1</v>
+      </c>
+      <c r="D9" s="46">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Asset turn over report -Mojodi completed
</commit_message>
<xml_diff>
--- a/Documents/Book1.xlsx
+++ b/Documents/Book1.xlsx
@@ -9,14 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="permissions" sheetId="4" r:id="rId4"/>
+    <sheet name="order page" sheetId="5" r:id="rId5"/>
+    <sheet name="sample" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">sample!$B$1:$E$28</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="84">
   <si>
     <t>دوربین</t>
   </si>
@@ -210,13 +215,82 @@
   </si>
   <si>
     <t>record_owner</t>
+  </si>
+  <si>
+    <t>new order</t>
+  </si>
+  <si>
+    <t>reload order</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>delete order</t>
+  </si>
+  <si>
+    <t>by venue</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>by admin</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>alvand</t>
+  </si>
+  <si>
+    <t>kados</t>
+  </si>
+  <si>
+    <t>sanaz</t>
+  </si>
+  <si>
+    <t>tabriz</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>headphone</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>radif</t>
+  </si>
+  <si>
+    <t>ahvaz</t>
+  </si>
+  <si>
+    <t>mashhad</t>
+  </si>
+  <si>
+    <t>sari</t>
+  </si>
+  <si>
+    <t>laptop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +309,26 @@
       <sz val="11.3"/>
       <color rgb="FFC3CEE3"/>
       <name val="Fira Code"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -599,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -693,6 +787,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1982,13 +2079,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
@@ -2320,4 +2417,717 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1">
+      <c r="A2" s="52">
+        <v>15</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="52">
+        <v>1</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+    </row>
+    <row r="3" spans="1:9" hidden="1">
+      <c r="A3" s="53">
+        <v>1</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="53">
+        <v>20</v>
+      </c>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+    </row>
+    <row r="4" spans="1:9" hidden="1">
+      <c r="A4" s="53">
+        <v>2</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="53">
+        <v>300</v>
+      </c>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" hidden="1">
+      <c r="A5" s="53">
+        <v>6</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53">
+        <v>50</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+    </row>
+    <row r="6" spans="1:9" hidden="1">
+      <c r="A6" s="53">
+        <v>8</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53">
+        <v>6</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+    </row>
+    <row r="7" spans="1:9" hidden="1">
+      <c r="A7" s="53">
+        <v>13</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53">
+        <v>2</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+    </row>
+    <row r="8" spans="1:9" hidden="1">
+      <c r="A8" s="52">
+        <v>22</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+    </row>
+    <row r="9" spans="1:9" hidden="1">
+      <c r="A9" s="52">
+        <v>25</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="53">
+        <v>10</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="53">
+        <v>100</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="53">
+        <v>12</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="53">
+        <v>5</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="52">
+        <v>26</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+    </row>
+    <row r="13" spans="1:9" hidden="1">
+      <c r="A13" s="52">
+        <v>17</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="52">
+        <v>1</v>
+      </c>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+    </row>
+    <row r="14" spans="1:9" hidden="1">
+      <c r="A14" s="52">
+        <v>21</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="52">
+        <v>100</v>
+      </c>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+    </row>
+    <row r="15" spans="1:9" hidden="1">
+      <c r="A15" s="53">
+        <v>3</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="53">
+        <v>10</v>
+      </c>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+    </row>
+    <row r="16" spans="1:9" hidden="1">
+      <c r="A16" s="53">
+        <v>4</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="53">
+        <v>200</v>
+      </c>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1">
+      <c r="A17" s="53">
+        <v>9</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53">
+        <v>4</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+    </row>
+    <row r="18" spans="1:9" hidden="1">
+      <c r="A18" s="53">
+        <v>11</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53">
+        <v>60</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1">
+      <c r="A19" s="53">
+        <v>14</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53">
+        <v>5</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+    </row>
+    <row r="20" spans="1:9" hidden="1">
+      <c r="A20" s="52">
+        <v>16</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+    </row>
+    <row r="21" spans="1:9" hidden="1">
+      <c r="A21" s="52">
+        <v>18</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+    </row>
+    <row r="22" spans="1:9" hidden="1">
+      <c r="A22" s="52">
+        <v>20</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+    </row>
+    <row r="23" spans="1:9" hidden="1">
+      <c r="A23" s="52">
+        <v>23</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1">
+      <c r="A24" s="52">
+        <v>27</v>
+      </c>
+      <c r="B24" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1">
+      <c r="A25" s="52">
+        <v>19</v>
+      </c>
+      <c r="B25" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="52">
+        <v>1</v>
+      </c>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+    </row>
+    <row r="26" spans="1:9" hidden="1">
+      <c r="A26" s="52">
+        <v>24</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="52">
+        <v>60</v>
+      </c>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+    </row>
+    <row r="27" spans="1:9" hidden="1">
+      <c r="A27" s="53">
+        <v>5</v>
+      </c>
+      <c r="B27" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="53">
+        <v>50</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:9" hidden="1">
+      <c r="A28" s="53">
+        <v>7</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="53">
+        <v>10</v>
+      </c>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:E28">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="kados"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:F28">
+    <sortCondition ref="B25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>